<commit_message>
Final Code - Thesis Daniel Rauser
</commit_message>
<xml_diff>
--- a/Data/Plants_EDP.xlsx
+++ b/Data/Plants_EDP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/darcor/PycharmProjects/Setup/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63C3D90-0EE5-4E4C-8882-7E1B9F338658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B44B28A-A544-EA40-B516-086CAD061EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18080" yWindow="1040" windowWidth="17760" windowHeight="21120" activeTab="3" xr2:uid="{F223C087-CA58-3841-BDD9-F0A772163B66}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="36000" windowHeight="22520" activeTab="5" xr2:uid="{F223C087-CA58-3841-BDD9-F0A772163B66}"/>
   </bookViews>
   <sheets>
     <sheet name="SOURCES" sheetId="2" r:id="rId1"/>
@@ -27,13 +27,13 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ALL!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Gas!$A$1:$H$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Hydro!$A$1:$J$58</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Photovoltaic!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Photovoltaic!$A$1:$J$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Plants!$A$1:$G$99</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Wind!$A$1:$O$88</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId10"/>
+    <pivotCache cacheId="0" r:id="rId10"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -203,7 +203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1643" uniqueCount="339">
   <si>
     <t>Plant Name</t>
   </si>
@@ -1217,12 +1217,18 @@
   </si>
   <si>
     <t>Ecotecnia 74</t>
+  </si>
+  <si>
+    <t>Activated</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1326,7 +1332,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1344,6 +1350,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1878,7 +1887,7 @@
       <xdr:rowOff>194953</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>171662</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>13490</xdr:rowOff>
@@ -1962,7 +1971,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>329927</xdr:colOff>
+      <xdr:colOff>548422</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>13943</xdr:rowOff>
     </xdr:to>
@@ -3204,7 +3213,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{06860CA4-1D34-824D-AEAE-3805E1E10A63}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{06860CA4-1D34-824D-AEAE-3805E1E10A63}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="">
   <location ref="D3:E7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -3284,7 +3293,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{38847370-BA2E-8843-B9A3-31372DE8F1E7}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{38847370-BA2E-8843-B9A3-31372DE8F1E7}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -6450,7 +6459,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
@@ -11732,7 +11741,7 @@
         <v>5200</v>
       </c>
       <c r="G60" s="2">
-        <f t="shared" ref="G60:G91" si="4">F60/1000</f>
+        <f t="shared" ref="G60:G88" si="4">F60/1000</f>
         <v>5.2</v>
       </c>
       <c r="H60" s="2">
@@ -13147,21 +13156,22 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79FE95B8-B3C1-7A45-AEFC-37FB3C2E14E3}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView zoomScale="93" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="43.83203125" customWidth="1"/>
-    <col min="5" max="5" width="21.5" customWidth="1"/>
-    <col min="6" max="6" width="31.83203125" customWidth="1"/>
-    <col min="9" max="9" width="59.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5" customWidth="1"/>
+    <col min="7" max="7" width="31.83203125" customWidth="1"/>
+    <col min="10" max="10" width="59.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13174,23 +13184,26 @@
       <c r="D1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>51</v>
       </c>
@@ -13203,31 +13216,34 @@
       <c r="D2" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="14">
+        <v>45352</v>
+      </c>
+      <c r="F2" s="2">
         <v>202</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>330</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <f>VALUE(MID(
-  I2,
-  SEARCH("/", I2, SEARCH("map=", I2) + 4) + 1,
-  SEARCH("/", I2, SEARCH("/", I2, SEARCH("map=", I2) + 4) + 1) - SEARCH("/", I2, SEARCH("map=", I2) + 4) - 1
+  J2,
+  SEARCH("/", J2, SEARCH("map=", J2) + 4) + 1,
+  SEARCH("/", J2, SEARCH("/", J2, SEARCH("map=", J2) + 4) + 1) - SEARCH("/", J2, SEARCH("map=", J2) + 4) - 1
 ))</f>
         <v>39.101799999999997</v>
       </c>
-      <c r="H2" s="2">
-        <f>VALUE(MID(I2,
-     SEARCH("/", I2, SEARCH("/", I2, SEARCH("map=", I2)+4)+1)+1,
-     LEN(I2) - SEARCH("/", I2, SEARCH("/", I2, SEARCH("map=", I2)+4)+1)))</f>
+      <c r="I2" s="2">
+        <f>VALUE(MID(J2,
+     SEARCH("/", J2, SEARCH("/", J2, SEARCH("map=", J2)+4)+1)+1,
+     LEN(J2) - SEARCH("/", J2, SEARCH("/", J2, SEARCH("map=", J2)+4)+1)))</f>
         <v>-8.8240999999999996</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>52</v>
       </c>
@@ -13240,29 +13256,30 @@
       <c r="D3" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="14"/>
+      <c r="F3" s="2">
         <v>189</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3">
-        <f t="shared" ref="G3:G12" si="0">VALUE(MID(
-  I3,
-  SEARCH("/", I3, SEARCH("map=", I3) + 4) + 1,
-  SEARCH("/", I3, SEARCH("/", I3, SEARCH("map=", I3) + 4) + 1) - SEARCH("/", I3, SEARCH("map=", I3) + 4) - 1
+      <c r="G3" s="2"/>
+      <c r="H3">
+        <f t="shared" ref="H3:H12" si="0">VALUE(MID(
+  J3,
+  SEARCH("/", J3, SEARCH("map=", J3) + 4) + 1,
+  SEARCH("/", J3, SEARCH("/", J3, SEARCH("map=", J3) + 4) + 1) - SEARCH("/", J3, SEARCH("map=", J3) + 4) - 1
 ))</f>
         <v>39.20778</v>
       </c>
-      <c r="H3" s="2">
-        <f t="shared" ref="H3:H12" si="1">VALUE(MID(I3,
-     SEARCH("/", I3, SEARCH("/", I3, SEARCH("map=", I3)+4)+1)+1,
-     LEN(I3) - SEARCH("/", I3, SEARCH("/", I3, SEARCH("map=", I3)+4)+1)))</f>
+      <c r="I3" s="2">
+        <f t="shared" ref="I3:I12" si="1">VALUE(MID(J3,
+     SEARCH("/", J3, SEARCH("/", J3, SEARCH("map=", J3)+4)+1)+1,
+     LEN(J3) - SEARCH("/", J3, SEARCH("/", J3, SEARCH("map=", J3)+4)+1)))</f>
         <v>-8.8079499999999999</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>54</v>
       </c>
@@ -13275,23 +13292,24 @@
       <c r="D4" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="14"/>
+      <c r="F4" s="2">
         <v>60</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4">
+      <c r="G4" s="2"/>
+      <c r="H4">
         <f t="shared" si="0"/>
         <v>37.668129999999998</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <f t="shared" si="1"/>
         <v>-8.1894500000000008</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>55</v>
       </c>
@@ -13304,23 +13322,24 @@
       <c r="D5" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="14"/>
+      <c r="F5" s="2">
         <v>32.89</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5">
+      <c r="G5" s="2"/>
+      <c r="H5">
         <f t="shared" si="0"/>
         <v>38.700209999999998</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <f t="shared" si="1"/>
         <v>-8.8900400000000008</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>82</v>
       </c>
@@ -13333,23 +13352,24 @@
       <c r="D6" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="14"/>
+      <c r="F6" s="2">
         <v>21</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6">
+      <c r="G6" s="2"/>
+      <c r="H6">
         <f t="shared" si="0"/>
         <v>39.996450000000003</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <f t="shared" si="1"/>
         <v>-8.40076</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>56</v>
       </c>
@@ -13362,23 +13382,24 @@
       <c r="D7" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="14"/>
+      <c r="F7" s="2">
         <v>12.72</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7">
+      <c r="G7" s="2"/>
+      <c r="H7">
         <f t="shared" si="0"/>
         <v>38.694989999999997</v>
       </c>
-      <c r="H7" s="2">
+      <c r="I7" s="2">
         <f t="shared" si="1"/>
         <v>-8.8931299999999993</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>91</v>
       </c>
@@ -13391,23 +13412,24 @@
       <c r="D8" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="14"/>
+      <c r="F8" s="2">
         <v>8.4</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8">
+      <c r="G8" s="2"/>
+      <c r="H8">
         <f t="shared" si="0"/>
         <v>40.308529999999998</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I8" s="2">
         <f t="shared" si="1"/>
         <v>-7.1445299999999996</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>57</v>
       </c>
@@ -13420,23 +13442,24 @@
       <c r="D9" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="14"/>
+      <c r="F9" s="2">
         <v>5</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9">
+      <c r="G9" s="2"/>
+      <c r="H9">
         <f t="shared" si="0"/>
         <v>38.199339000000002</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I9" s="2">
         <f t="shared" si="1"/>
         <v>-7.497547</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>60</v>
       </c>
@@ -13449,23 +13472,24 @@
       <c r="D10" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="14"/>
+      <c r="F10" s="2">
         <v>3</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10">
+      <c r="G10" s="2"/>
+      <c r="H10">
         <f t="shared" si="0"/>
         <v>37.076839999999997</v>
       </c>
-      <c r="H10" s="2">
+      <c r="I10" s="2">
         <f t="shared" si="1"/>
         <v>-7.8566599999999998</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>59</v>
       </c>
@@ -13478,23 +13502,24 @@
       <c r="D11" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="14"/>
+      <c r="F11" s="2">
         <v>2.6</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11">
+      <c r="G11" s="2"/>
+      <c r="H11">
         <f t="shared" si="0"/>
         <v>40.064196000000003</v>
       </c>
-      <c r="H11" s="2">
+      <c r="I11" s="2">
         <f t="shared" si="1"/>
         <v>-8.8526089999999993</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>58</v>
       </c>
@@ -13507,24 +13532,25 @@
       <c r="D12" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="14"/>
+      <c r="F12" s="2">
         <v>2.48</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12">
+      <c r="G12" s="2"/>
+      <c r="H12">
         <f t="shared" si="0"/>
         <v>40.824145000000001</v>
       </c>
-      <c r="H12" s="2">
+      <c r="I12" s="2">
         <f t="shared" si="1"/>
         <v>-8.5553460000000001</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>257</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1" xr:uid="{79FE95B8-B3C1-7A45-AEFC-37FB3C2E14E3}"/>
+  <autoFilter ref="A1:J1" xr:uid="{79FE95B8-B3C1-7A45-AEFC-37FB3C2E14E3}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -13535,7 +13561,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>